<commit_message>
renaming par output to apar and running some more tests.
#43
</commit_message>
<xml_diff>
--- a/pkg/data-raw/info.default.xlsx
+++ b/pkg/data-raw/info.default.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PG/pkg/data-raw/internal_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/Research/software/r3PG/pkg/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B96B081-98D1-7E4A-BB5D-E84C2BD40C0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F69C00-1A31-0D4B-AE90-B60C879C3EB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="2" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
   </bookViews>
@@ -1451,9 +1451,6 @@
     <t>NPP</t>
   </si>
   <si>
-    <t>par</t>
-  </si>
-  <si>
     <t>Total solar radiation (PAR) intercepted by canopy</t>
   </si>
   <si>
@@ -1998,6 +1995,9 @@
   </si>
   <si>
     <t>var_10_15</t>
+  </si>
+  <si>
+    <t>apar</t>
   </si>
 </sst>
 </file>
@@ -3984,8 +3984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3706E6-9BD2-3A49-A255-D2B55C8D9AB1}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5627,19 +5627,19 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>474</v>
+        <v>656</v>
       </c>
       <c r="D79" t="s">
         <v>468</v>
       </c>
       <c r="E79" t="s">
+        <v>474</v>
+      </c>
+      <c r="F79" t="s">
         <v>475</v>
       </c>
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>476</v>
-      </c>
-      <c r="G79" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -5650,19 +5650,19 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D80" t="s">
         <v>468</v>
       </c>
       <c r="E80" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F80" t="s">
         <v>128</v>
       </c>
       <c r="G80" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -5673,19 +5673,19 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D81" t="s">
         <v>468</v>
       </c>
       <c r="E81" t="s">
+        <v>480</v>
+      </c>
+      <c r="F81" t="s">
         <v>481</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>482</v>
-      </c>
-      <c r="G81" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -5696,19 +5696,19 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D82" t="s">
         <v>468</v>
       </c>
       <c r="E82" t="s">
+        <v>484</v>
+      </c>
+      <c r="F82" t="s">
         <v>485</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>486</v>
-      </c>
-      <c r="G82" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -5719,19 +5719,19 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D83" t="s">
         <v>468</v>
       </c>
       <c r="E83" t="s">
+        <v>488</v>
+      </c>
+      <c r="F83" t="s">
+        <v>485</v>
+      </c>
+      <c r="G83" t="s">
         <v>489</v>
-      </c>
-      <c r="F83" t="s">
-        <v>486</v>
-      </c>
-      <c r="G83" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -5742,19 +5742,19 @@
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D84" t="s">
         <v>468</v>
       </c>
       <c r="E84" t="s">
+        <v>491</v>
+      </c>
+      <c r="F84" t="s">
+        <v>485</v>
+      </c>
+      <c r="G84" t="s">
         <v>492</v>
-      </c>
-      <c r="F84" t="s">
-        <v>486</v>
-      </c>
-      <c r="G84" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -5765,19 +5765,19 @@
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D85" t="s">
         <v>468</v>
       </c>
       <c r="E85" t="s">
+        <v>494</v>
+      </c>
+      <c r="F85" t="s">
+        <v>128</v>
+      </c>
+      <c r="G85" t="s">
         <v>495</v>
-      </c>
-      <c r="F85" t="s">
-        <v>128</v>
-      </c>
-      <c r="G85" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -5788,19 +5788,19 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D86" t="s">
         <v>468</v>
       </c>
       <c r="E86" t="s">
+        <v>497</v>
+      </c>
+      <c r="F86" t="s">
+        <v>128</v>
+      </c>
+      <c r="G86" t="s">
         <v>498</v>
-      </c>
-      <c r="F86" t="s">
-        <v>128</v>
-      </c>
-      <c r="G86" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -5811,19 +5811,19 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D87" t="s">
         <v>468</v>
       </c>
       <c r="E87" t="s">
+        <v>500</v>
+      </c>
+      <c r="F87" t="s">
+        <v>128</v>
+      </c>
+      <c r="G87" t="s">
         <v>501</v>
-      </c>
-      <c r="F87" t="s">
-        <v>128</v>
-      </c>
-      <c r="G87" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -5834,19 +5834,19 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D88" t="s">
         <v>468</v>
       </c>
       <c r="E88" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F88" t="s">
         <v>128</v>
       </c>
       <c r="G88" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -5857,19 +5857,19 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D89" t="s">
         <v>468</v>
       </c>
       <c r="E89" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F89" t="s">
         <v>391</v>
       </c>
       <c r="G89" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -5880,7 +5880,7 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D90" t="s">
         <v>468</v>
@@ -5894,7 +5894,7 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D91" t="s">
         <v>468</v>
@@ -5908,19 +5908,19 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
+        <v>509</v>
+      </c>
+      <c r="D92" t="s">
         <v>510</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>511</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>512</v>
       </c>
-      <c r="F92" t="s">
-        <v>513</v>
-      </c>
       <c r="G92" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -5931,19 +5931,19 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
+        <v>513</v>
+      </c>
+      <c r="D93" t="s">
+        <v>510</v>
+      </c>
+      <c r="E93" t="s">
         <v>514</v>
       </c>
-      <c r="D93" t="s">
-        <v>511</v>
-      </c>
-      <c r="E93" t="s">
-        <v>515</v>
-      </c>
       <c r="F93" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G93" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -5954,19 +5954,19 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
+        <v>515</v>
+      </c>
+      <c r="D94" t="s">
+        <v>510</v>
+      </c>
+      <c r="E94" t="s">
         <v>516</v>
       </c>
-      <c r="D94" t="s">
-        <v>511</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>517</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>518</v>
-      </c>
-      <c r="G94" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -5977,19 +5977,19 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
+        <v>519</v>
+      </c>
+      <c r="D95" t="s">
+        <v>510</v>
+      </c>
+      <c r="E95" t="s">
         <v>520</v>
       </c>
-      <c r="D95" t="s">
-        <v>511</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>521</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>522</v>
-      </c>
-      <c r="G95" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -6000,19 +6000,19 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
+        <v>523</v>
+      </c>
+      <c r="D96" t="s">
+        <v>510</v>
+      </c>
+      <c r="E96" t="s">
         <v>524</v>
       </c>
-      <c r="D96" t="s">
-        <v>511</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
+        <v>128</v>
+      </c>
+      <c r="G96" t="s">
         <v>525</v>
-      </c>
-      <c r="F96" t="s">
-        <v>128</v>
-      </c>
-      <c r="G96" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -6023,19 +6023,19 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
+        <v>526</v>
+      </c>
+      <c r="D97" t="s">
+        <v>510</v>
+      </c>
+      <c r="E97" t="s">
         <v>527</v>
       </c>
-      <c r="D97" t="s">
-        <v>511</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
+        <v>521</v>
+      </c>
+      <c r="G97" t="s">
         <v>528</v>
-      </c>
-      <c r="F97" t="s">
-        <v>522</v>
-      </c>
-      <c r="G97" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -6046,19 +6046,19 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
+        <v>529</v>
+      </c>
+      <c r="D98" t="s">
+        <v>510</v>
+      </c>
+      <c r="E98" t="s">
         <v>530</v>
       </c>
-      <c r="D98" t="s">
-        <v>511</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
+        <v>521</v>
+      </c>
+      <c r="G98" t="s">
         <v>531</v>
-      </c>
-      <c r="F98" t="s">
-        <v>522</v>
-      </c>
-      <c r="G98" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -6069,19 +6069,19 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
+        <v>532</v>
+      </c>
+      <c r="D99" t="s">
+        <v>510</v>
+      </c>
+      <c r="E99" t="s">
         <v>533</v>
       </c>
-      <c r="D99" t="s">
-        <v>511</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>534</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>535</v>
-      </c>
-      <c r="G99" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -6092,19 +6092,19 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
+        <v>536</v>
+      </c>
+      <c r="D100" t="s">
+        <v>510</v>
+      </c>
+      <c r="E100" t="s">
         <v>537</v>
       </c>
-      <c r="D100" t="s">
-        <v>511</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
+        <v>534</v>
+      </c>
+      <c r="G100" t="s">
         <v>538</v>
-      </c>
-      <c r="F100" t="s">
-        <v>535</v>
-      </c>
-      <c r="G100" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -6115,19 +6115,19 @@
         <v>10</v>
       </c>
       <c r="C101" t="s">
+        <v>539</v>
+      </c>
+      <c r="D101" t="s">
+        <v>510</v>
+      </c>
+      <c r="E101" t="s">
         <v>540</v>
       </c>
-      <c r="D101" t="s">
-        <v>511</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
+        <v>517</v>
+      </c>
+      <c r="G101" t="s">
         <v>541</v>
-      </c>
-      <c r="F101" t="s">
-        <v>518</v>
-      </c>
-      <c r="G101" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -6138,19 +6138,19 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
+        <v>542</v>
+      </c>
+      <c r="D102" t="s">
+        <v>510</v>
+      </c>
+      <c r="E102" t="s">
         <v>543</v>
       </c>
-      <c r="D102" t="s">
-        <v>511</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
+        <v>517</v>
+      </c>
+      <c r="G102" t="s">
         <v>544</v>
-      </c>
-      <c r="F102" t="s">
-        <v>518</v>
-      </c>
-      <c r="G102" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -6161,19 +6161,19 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
+        <v>545</v>
+      </c>
+      <c r="D103" t="s">
+        <v>510</v>
+      </c>
+      <c r="E103" t="s">
         <v>546</v>
       </c>
-      <c r="D103" t="s">
-        <v>511</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
+        <v>521</v>
+      </c>
+      <c r="G103" t="s">
         <v>547</v>
-      </c>
-      <c r="F103" t="s">
-        <v>522</v>
-      </c>
-      <c r="G103" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -6184,19 +6184,19 @@
         <v>13</v>
       </c>
       <c r="C104" t="s">
+        <v>548</v>
+      </c>
+      <c r="D104" t="s">
+        <v>510</v>
+      </c>
+      <c r="E104" t="s">
         <v>549</v>
       </c>
-      <c r="D104" t="s">
-        <v>511</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
+        <v>521</v>
+      </c>
+      <c r="G104" t="s">
         <v>550</v>
-      </c>
-      <c r="F104" t="s">
-        <v>522</v>
-      </c>
-      <c r="G104" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -6207,10 +6207,10 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D105" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -6221,10 +6221,10 @@
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D106" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -6235,19 +6235,19 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
+        <v>553</v>
+      </c>
+      <c r="D107" t="s">
         <v>554</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>555</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>556</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>557</v>
-      </c>
-      <c r="G107" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -6258,19 +6258,19 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
+        <v>558</v>
+      </c>
+      <c r="D108" t="s">
+        <v>554</v>
+      </c>
+      <c r="E108" t="s">
         <v>559</v>
       </c>
-      <c r="D108" t="s">
-        <v>555</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>560</v>
       </c>
-      <c r="F108" t="s">
-        <v>561</v>
-      </c>
       <c r="G108" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -6281,19 +6281,19 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
+        <v>561</v>
+      </c>
+      <c r="D109" t="s">
+        <v>554</v>
+      </c>
+      <c r="E109" t="s">
         <v>562</v>
-      </c>
-      <c r="D109" t="s">
-        <v>555</v>
-      </c>
-      <c r="E109" t="s">
-        <v>563</v>
       </c>
       <c r="F109" t="s">
         <v>305</v>
       </c>
       <c r="G109" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -6304,19 +6304,19 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
+        <v>564</v>
+      </c>
+      <c r="D110" t="s">
+        <v>554</v>
+      </c>
+      <c r="E110" t="s">
         <v>565</v>
-      </c>
-      <c r="D110" t="s">
-        <v>555</v>
-      </c>
-      <c r="E110" t="s">
-        <v>566</v>
       </c>
       <c r="F110" t="s">
         <v>305</v>
       </c>
       <c r="G110" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -6327,10 +6327,10 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D111" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -6341,19 +6341,19 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
+        <v>568</v>
+      </c>
+      <c r="D112" t="s">
+        <v>554</v>
+      </c>
+      <c r="E112" t="s">
         <v>569</v>
-      </c>
-      <c r="D112" t="s">
-        <v>555</v>
-      </c>
-      <c r="E112" t="s">
-        <v>570</v>
       </c>
       <c r="F112" t="s">
         <v>333</v>
       </c>
       <c r="G112" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -6364,10 +6364,10 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D113" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -6378,19 +6378,19 @@
         <v>8</v>
       </c>
       <c r="C114" t="s">
+        <v>572</v>
+      </c>
+      <c r="D114" t="s">
+        <v>554</v>
+      </c>
+      <c r="E114" t="s">
         <v>573</v>
-      </c>
-      <c r="D114" t="s">
-        <v>555</v>
-      </c>
-      <c r="E114" t="s">
-        <v>574</v>
       </c>
       <c r="F114" t="s">
         <v>305</v>
       </c>
       <c r="G114" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -6401,10 +6401,10 @@
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D115" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E115" t="s">
         <v>316</v>
@@ -6413,7 +6413,7 @@
         <v>317</v>
       </c>
       <c r="G115" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -6424,10 +6424,10 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D116" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E116" t="s">
         <v>308</v>
@@ -6436,7 +6436,7 @@
         <v>309</v>
       </c>
       <c r="G116" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -6447,10 +6447,10 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D117" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E117" t="s">
         <v>332</v>
@@ -6459,7 +6459,7 @@
         <v>333</v>
       </c>
       <c r="G117" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -6470,10 +6470,10 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D118" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E118" t="s">
         <v>319</v>
@@ -6482,7 +6482,7 @@
         <v>320</v>
       </c>
       <c r="G118" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -6493,10 +6493,10 @@
         <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D119" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E119" t="s">
         <v>390</v>
@@ -6505,7 +6505,7 @@
         <v>391</v>
       </c>
       <c r="G119" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -6516,10 +6516,10 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D120" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -6530,10 +6530,10 @@
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D121" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -6544,19 +6544,19 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
+        <v>587</v>
+      </c>
+      <c r="D122" t="s">
         <v>588</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
         <v>589</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>590</v>
       </c>
-      <c r="F122" t="s">
+      <c r="G122" t="s">
         <v>591</v>
-      </c>
-      <c r="G122" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -6567,19 +6567,19 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
+        <v>592</v>
+      </c>
+      <c r="D123" t="s">
+        <v>588</v>
+      </c>
+      <c r="E123" t="s">
         <v>593</v>
       </c>
-      <c r="D123" t="s">
-        <v>589</v>
-      </c>
-      <c r="E123" t="s">
+      <c r="F123" t="s">
+        <v>590</v>
+      </c>
+      <c r="G123" t="s">
         <v>594</v>
-      </c>
-      <c r="F123" t="s">
-        <v>591</v>
-      </c>
-      <c r="G123" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -6590,16 +6590,16 @@
         <v>3</v>
       </c>
       <c r="C124" t="s">
+        <v>595</v>
+      </c>
+      <c r="D124" t="s">
+        <v>588</v>
+      </c>
+      <c r="E124" t="s">
         <v>596</v>
       </c>
-      <c r="D124" t="s">
-        <v>589</v>
-      </c>
-      <c r="E124" t="s">
-        <v>597</v>
-      </c>
       <c r="G124" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -6610,16 +6610,16 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
+        <v>597</v>
+      </c>
+      <c r="D125" t="s">
+        <v>588</v>
+      </c>
+      <c r="E125" t="s">
         <v>598</v>
       </c>
-      <c r="D125" t="s">
-        <v>589</v>
-      </c>
-      <c r="E125" t="s">
-        <v>599</v>
-      </c>
       <c r="G125" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -6630,19 +6630,19 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
+        <v>599</v>
+      </c>
+      <c r="D126" t="s">
+        <v>588</v>
+      </c>
+      <c r="E126" t="s">
         <v>600</v>
-      </c>
-      <c r="D126" t="s">
-        <v>589</v>
-      </c>
-      <c r="E126" t="s">
-        <v>601</v>
       </c>
       <c r="F126" t="s">
         <v>288</v>
       </c>
       <c r="G126" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -6653,10 +6653,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D127" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
@@ -6667,10 +6667,10 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D128" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
@@ -6681,10 +6681,10 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D129" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
@@ -6695,10 +6695,10 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D130" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
@@ -6709,10 +6709,10 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D131" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -6723,10 +6723,10 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D132" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -6737,10 +6737,10 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D133" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -6751,10 +6751,10 @@
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D134" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -6765,10 +6765,10 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D135" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -6779,10 +6779,10 @@
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D136" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -6793,19 +6793,19 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
+        <v>612</v>
+      </c>
+      <c r="D137" t="s">
         <v>613</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" t="s">
         <v>614</v>
       </c>
-      <c r="E137" t="s">
+      <c r="F137" t="s">
+        <v>128</v>
+      </c>
+      <c r="G137" t="s">
         <v>615</v>
-      </c>
-      <c r="F137" t="s">
-        <v>128</v>
-      </c>
-      <c r="G137" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -6816,19 +6816,19 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
+        <v>616</v>
+      </c>
+      <c r="D138" t="s">
+        <v>613</v>
+      </c>
+      <c r="E138" t="s">
         <v>617</v>
       </c>
-      <c r="D138" t="s">
-        <v>614</v>
-      </c>
-      <c r="E138" t="s">
+      <c r="F138" t="s">
+        <v>128</v>
+      </c>
+      <c r="G138" t="s">
         <v>618</v>
-      </c>
-      <c r="F138" t="s">
-        <v>128</v>
-      </c>
-      <c r="G138" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -6839,19 +6839,19 @@
         <v>3</v>
       </c>
       <c r="C139" t="s">
+        <v>619</v>
+      </c>
+      <c r="D139" t="s">
+        <v>613</v>
+      </c>
+      <c r="E139" t="s">
         <v>620</v>
       </c>
-      <c r="D139" t="s">
-        <v>614</v>
-      </c>
-      <c r="E139" t="s">
+      <c r="F139" t="s">
+        <v>128</v>
+      </c>
+      <c r="G139" t="s">
         <v>621</v>
-      </c>
-      <c r="F139" t="s">
-        <v>128</v>
-      </c>
-      <c r="G139" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -6862,19 +6862,19 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
+        <v>622</v>
+      </c>
+      <c r="D140" t="s">
+        <v>613</v>
+      </c>
+      <c r="E140" t="s">
         <v>623</v>
       </c>
-      <c r="D140" t="s">
-        <v>614</v>
-      </c>
-      <c r="E140" t="s">
+      <c r="F140" t="s">
+        <v>128</v>
+      </c>
+      <c r="G140" t="s">
         <v>624</v>
-      </c>
-      <c r="F140" t="s">
-        <v>128</v>
-      </c>
-      <c r="G140" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
@@ -6885,19 +6885,19 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
+        <v>625</v>
+      </c>
+      <c r="D141" t="s">
+        <v>613</v>
+      </c>
+      <c r="E141" t="s">
         <v>626</v>
       </c>
-      <c r="D141" t="s">
-        <v>614</v>
-      </c>
-      <c r="E141" t="s">
+      <c r="F141" t="s">
+        <v>128</v>
+      </c>
+      <c r="G141" t="s">
         <v>627</v>
-      </c>
-      <c r="F141" t="s">
-        <v>128</v>
-      </c>
-      <c r="G141" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
@@ -6908,19 +6908,19 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
+        <v>628</v>
+      </c>
+      <c r="D142" t="s">
+        <v>613</v>
+      </c>
+      <c r="E142" t="s">
         <v>629</v>
       </c>
-      <c r="D142" t="s">
-        <v>614</v>
-      </c>
-      <c r="E142" t="s">
+      <c r="F142" t="s">
+        <v>128</v>
+      </c>
+      <c r="G142" t="s">
         <v>630</v>
-      </c>
-      <c r="F142" t="s">
-        <v>128</v>
-      </c>
-      <c r="G142" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -6931,19 +6931,19 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
+        <v>631</v>
+      </c>
+      <c r="D143" t="s">
+        <v>613</v>
+      </c>
+      <c r="E143" t="s">
         <v>632</v>
-      </c>
-      <c r="D143" t="s">
-        <v>614</v>
-      </c>
-      <c r="E143" t="s">
-        <v>633</v>
       </c>
       <c r="F143" t="s">
         <v>367</v>
       </c>
       <c r="G143" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -6954,19 +6954,19 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
+        <v>634</v>
+      </c>
+      <c r="D144" t="s">
+        <v>613</v>
+      </c>
+      <c r="E144" t="s">
         <v>635</v>
-      </c>
-      <c r="D144" t="s">
-        <v>614</v>
-      </c>
-      <c r="E144" t="s">
-        <v>636</v>
       </c>
       <c r="F144" t="s">
         <v>367</v>
       </c>
       <c r="G144" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
@@ -6977,19 +6977,19 @@
         <v>9</v>
       </c>
       <c r="C145" t="s">
+        <v>637</v>
+      </c>
+      <c r="D145" t="s">
+        <v>613</v>
+      </c>
+      <c r="E145" t="s">
         <v>638</v>
-      </c>
-      <c r="D145" t="s">
-        <v>614</v>
-      </c>
-      <c r="E145" t="s">
-        <v>639</v>
       </c>
       <c r="F145" t="s">
         <v>367</v>
       </c>
       <c r="G145" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
@@ -7000,19 +7000,19 @@
         <v>10</v>
       </c>
       <c r="C146" t="s">
+        <v>640</v>
+      </c>
+      <c r="D146" t="s">
+        <v>613</v>
+      </c>
+      <c r="E146" t="s">
         <v>641</v>
-      </c>
-      <c r="D146" t="s">
-        <v>614</v>
-      </c>
-      <c r="E146" t="s">
-        <v>642</v>
       </c>
       <c r="F146" t="s">
         <v>367</v>
       </c>
       <c r="G146" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
@@ -7023,19 +7023,19 @@
         <v>11</v>
       </c>
       <c r="C147" t="s">
+        <v>643</v>
+      </c>
+      <c r="D147" t="s">
+        <v>613</v>
+      </c>
+      <c r="E147" t="s">
         <v>644</v>
-      </c>
-      <c r="D147" t="s">
-        <v>614</v>
-      </c>
-      <c r="E147" t="s">
-        <v>645</v>
       </c>
       <c r="F147" t="s">
         <v>367</v>
       </c>
       <c r="G147" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
@@ -7046,19 +7046,19 @@
         <v>12</v>
       </c>
       <c r="C148" t="s">
+        <v>646</v>
+      </c>
+      <c r="D148" t="s">
+        <v>613</v>
+      </c>
+      <c r="E148" t="s">
         <v>647</v>
-      </c>
-      <c r="D148" t="s">
-        <v>614</v>
-      </c>
-      <c r="E148" t="s">
-        <v>648</v>
       </c>
       <c r="F148" t="s">
         <v>367</v>
       </c>
       <c r="G148" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
@@ -7069,19 +7069,19 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
+        <v>649</v>
+      </c>
+      <c r="D149" t="s">
+        <v>613</v>
+      </c>
+      <c r="E149" t="s">
         <v>650</v>
-      </c>
-      <c r="D149" t="s">
-        <v>614</v>
-      </c>
-      <c r="E149" t="s">
-        <v>651</v>
       </c>
       <c r="F149" t="s">
         <v>367</v>
       </c>
       <c r="G149" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -7092,19 +7092,19 @@
         <v>14</v>
       </c>
       <c r="C150" t="s">
+        <v>652</v>
+      </c>
+      <c r="D150" t="s">
+        <v>613</v>
+      </c>
+      <c r="E150" t="s">
         <v>653</v>
-      </c>
-      <c r="D150" t="s">
-        <v>614</v>
-      </c>
-      <c r="E150" t="s">
-        <v>654</v>
       </c>
       <c r="F150" t="s">
         <v>367</v>
       </c>
       <c r="G150" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
@@ -7115,10 +7115,10 @@
         <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D151" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>